<commit_message>
Create linked list data structure
</commit_message>
<xml_diff>
--- a/Data_bases/Odczyt_z_pliku.xlsx
+++ b/Data_bases/Odczyt_z_pliku.xlsx
@@ -423,47 +423,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -473,222 +473,222 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55">
@@ -698,17 +698,17 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
@@ -718,37 +718,37 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -758,162 +758,162 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>